<commit_message>
rework new hero model
</commit_message>
<xml_diff>
--- a/Provinence3/ART.xlsx
+++ b/Provinence3/ART.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7305" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="2D" sheetId="1" r:id="rId1"/>
@@ -362,9 +362,6 @@
     <t>2 уровень</t>
   </si>
   <si>
-    <t>Типа для всего. Скрепы и все такое</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Splinter</t>
   </si>
   <si>
@@ -374,15 +371,6 @@
     <t>Рецепт</t>
   </si>
   <si>
-    <t>Броня</t>
-  </si>
-  <si>
-    <t>Оружие</t>
-  </si>
-  <si>
-    <t>Талисман</t>
-  </si>
-  <si>
     <t>Раскрытый свиток на которм изображен соотвествующий символ</t>
   </si>
   <si>
@@ -540,6 +528,18 @@
   </si>
   <si>
     <t>http://jjpeabody.deviantart.com/art/Mysterious-Desert-472797577?q=favby%3AKurman%2F51352955&amp;qo=630</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Типа для всего. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Броня</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Оружие</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Талисман</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +600,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -698,7 +710,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -729,6 +741,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -759,12 +777,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
@@ -1050,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1108,7 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="30" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
@@ -1131,7 +1150,7 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="31" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="s">
@@ -1145,7 +1164,7 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C8" t="s">
@@ -1159,7 +1178,7 @@
       <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="31" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
@@ -1173,7 +1192,7 @@
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="31" t="s">
         <v>24</v>
       </c>
       <c r="C10" t="s">
@@ -1187,7 +1206,7 @@
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C11" t="s">
@@ -1241,10 +1260,10 @@
       <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="27" t="s">
         <v>38</v>
       </c>
       <c r="D15">
@@ -1255,8 +1274,8 @@
       <c r="A16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="28"/>
       <c r="D16">
         <v>0</v>
       </c>
@@ -1265,8 +1284,8 @@
       <c r="A17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="26"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="28"/>
       <c r="D17">
         <v>0</v>
       </c>
@@ -1275,8 +1294,8 @@
       <c r="A18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="26"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="28"/>
       <c r="D18">
         <v>0</v>
       </c>
@@ -1285,8 +1304,8 @@
       <c r="A19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="26"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="28"/>
       <c r="D19">
         <v>0</v>
       </c>
@@ -1295,8 +1314,8 @@
       <c r="A20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="27"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="29"/>
       <c r="D20">
         <v>0</v>
       </c>
@@ -1319,10 +1338,10 @@
       <c r="A22" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="19" t="s">
         <v>44</v>
       </c>
       <c r="D22">
@@ -1333,8 +1352,8 @@
       <c r="A23" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
       <c r="D23">
         <v>0</v>
       </c>
@@ -1343,8 +1362,8 @@
       <c r="A24" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="28"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
       <c r="D24">
         <v>0</v>
       </c>
@@ -1357,7 +1376,7 @@
         <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1367,7 +1386,7 @@
       <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="31" t="s">
         <v>51</v>
       </c>
       <c r="D26">
@@ -1390,7 +1409,7 @@
       <c r="B28" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="26" t="s">
         <v>83</v>
       </c>
       <c r="D28">
@@ -1404,7 +1423,7 @@
       <c r="B29" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="19"/>
+      <c r="C29" s="21"/>
       <c r="D29">
         <v>1</v>
       </c>
@@ -1416,7 +1435,7 @@
       <c r="B30" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="19"/>
+      <c r="C30" s="21"/>
       <c r="D30">
         <v>0</v>
       </c>
@@ -1428,7 +1447,7 @@
       <c r="B31" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="19"/>
+      <c r="C31" s="21"/>
       <c r="D31">
         <v>0</v>
       </c>
@@ -1440,7 +1459,7 @@
       <c r="B32" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="19"/>
+      <c r="C32" s="21"/>
       <c r="D32">
         <v>0</v>
       </c>
@@ -1452,7 +1471,7 @@
       <c r="B33" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="19"/>
+      <c r="C33" s="21"/>
       <c r="D33">
         <v>0</v>
       </c>
@@ -1464,7 +1483,7 @@
       <c r="B34" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="19"/>
+      <c r="C34" s="21"/>
       <c r="D34">
         <v>0</v>
       </c>
@@ -1476,7 +1495,7 @@
       <c r="B35" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="19"/>
+      <c r="C35" s="21"/>
       <c r="D35">
         <v>0</v>
       </c>
@@ -1488,7 +1507,7 @@
       <c r="B36" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="19"/>
+      <c r="C36" s="21"/>
       <c r="D36">
         <v>0</v>
       </c>
@@ -1500,7 +1519,7 @@
       <c r="B37" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="19"/>
+      <c r="C37" s="21"/>
       <c r="D37">
         <v>0</v>
       </c>
@@ -1512,7 +1531,7 @@
       <c r="B38" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="20"/>
+      <c r="C38" s="22"/>
       <c r="D38">
         <v>0</v>
       </c>
@@ -1531,11 +1550,11 @@
       <c r="A40" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="19" t="s">
-        <v>112</v>
+      <c r="C40" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1545,8 +1564,8 @@
       <c r="A41" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
       <c r="D41">
         <v>0</v>
       </c>
@@ -1555,8 +1574,8 @@
       <c r="A42" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
       <c r="D42">
         <v>0</v>
       </c>
@@ -1565,8 +1584,8 @@
       <c r="A43" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="21"/>
       <c r="D43">
         <v>0</v>
       </c>
@@ -1574,7 +1593,7 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="11"/>
-      <c r="C44" s="19"/>
+      <c r="C44" s="21"/>
       <c r="D44">
         <v>0</v>
       </c>
@@ -1583,10 +1602,10 @@
       <c r="A45" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C45" s="19"/>
+      <c r="C45" s="21"/>
       <c r="D45">
         <v>0</v>
       </c>
@@ -1595,8 +1614,8 @@
       <c r="A46" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="19"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="21"/>
       <c r="D46">
         <v>0</v>
       </c>
@@ -1605,8 +1624,8 @@
       <c r="A47" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="19"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21"/>
       <c r="D47">
         <v>0</v>
       </c>
@@ -1615,8 +1634,8 @@
       <c r="A48" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="19"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="21"/>
       <c r="D48">
         <v>0</v>
       </c>
@@ -1624,32 +1643,32 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="11"/>
-      <c r="C49" s="19"/>
+      <c r="C49" s="21"/>
       <c r="D49">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C50" s="20"/>
+        <v>166</v>
+      </c>
+      <c r="C50" s="22"/>
       <c r="D50">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B51" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B51" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>118</v>
+      <c r="C51" s="26" t="s">
+        <v>114</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -1657,40 +1676,40 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
-        <v>114</v>
+        <v>167</v>
       </c>
       <c r="B52" s="11"/>
-      <c r="C52" s="19"/>
+      <c r="C52" s="21"/>
       <c r="D52">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
-        <v>115</v>
+        <v>168</v>
       </c>
       <c r="B53" s="11"/>
-      <c r="C53" s="19"/>
+      <c r="C53" s="21"/>
       <c r="D53">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>116</v>
+        <v>169</v>
       </c>
       <c r="B54" s="1"/>
-      <c r="C54" s="20"/>
+      <c r="C54" s="22"/>
       <c r="D54">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -1698,13 +1717,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B56" t="s">
-        <v>129</v>
-      </c>
-      <c r="C56" s="29" t="s">
-        <v>139</v>
+        <v>125</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>135</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -1712,109 +1731,109 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B57" t="s">
-        <v>131</v>
-      </c>
-      <c r="C57" s="29"/>
+        <v>127</v>
+      </c>
+      <c r="C57" s="18"/>
       <c r="D57">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B58" t="s">
-        <v>132</v>
-      </c>
-      <c r="C58" s="29"/>
+        <v>128</v>
+      </c>
+      <c r="C58" s="18"/>
       <c r="D58">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B59" t="s">
-        <v>133</v>
-      </c>
-      <c r="C59" s="29"/>
+        <v>129</v>
+      </c>
+      <c r="C59" s="18"/>
       <c r="D59">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>134</v>
-      </c>
-      <c r="C60" s="29"/>
+        <v>130</v>
+      </c>
+      <c r="C60" s="18"/>
       <c r="D60">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>135</v>
-      </c>
-      <c r="C61" s="29"/>
+        <v>131</v>
+      </c>
+      <c r="C61" s="18"/>
       <c r="D61">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B62" t="s">
-        <v>136</v>
-      </c>
-      <c r="C62" s="29"/>
+        <v>132</v>
+      </c>
+      <c r="C62" s="18"/>
       <c r="D62">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>137</v>
-      </c>
-      <c r="C63" s="29"/>
+        <v>133</v>
+      </c>
+      <c r="C63" s="18"/>
       <c r="D63">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B64" t="s">
-        <v>138</v>
-      </c>
-      <c r="C64" s="29"/>
+        <v>134</v>
+      </c>
+      <c r="C64" s="18"/>
       <c r="D64">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" s="19" t="s">
         <v>141</v>
-      </c>
-      <c r="B66" t="s">
-        <v>142</v>
-      </c>
-      <c r="C66" s="28" t="s">
-        <v>145</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -1822,44 +1841,51 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>144</v>
-      </c>
-      <c r="C67" s="28"/>
+        <v>140</v>
+      </c>
+      <c r="C67" s="19"/>
       <c r="D67">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>146</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="B69" s="32"/>
       <c r="C69" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>148</v>
-      </c>
-      <c r="B71" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="C71" s="29" t="s">
-        <v>151</v>
+        <v>144</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>149</v>
-      </c>
-      <c r="B72" s="29"/>
-      <c r="C72" s="29"/>
+        <v>145</v>
+      </c>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C28:C38"/>
     <mergeCell ref="C56:C64"/>
     <mergeCell ref="C66:C67"/>
     <mergeCell ref="B71:B72"/>
@@ -1867,12 +1893,6 @@
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="C40:C50"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C28:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1882,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1942,10 +1962,10 @@
       <c r="A7" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="18" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1953,15 +1973,15 @@
       <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2011,90 +2031,90 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B29" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B34" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B37" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B39" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>